<commit_message>
failed report index param
</commit_message>
<xml_diff>
--- a/files/ConduitLoginTest.xlsx
+++ b/files/ConduitLoginTest.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\WesamM\Desktop\automation-project\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{660E17CD-C750-4727-8715-69306021C082}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1610800-BCB8-4B67-9A5B-4AD4749FBA8F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{25638125-3395-45A5-9F15-6A89ADD712B7}"/>
+    <workbookView xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="11385" xr2:uid="{25638125-3395-45A5-9F15-6A89ADD712B7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet0" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="10">
   <si>
     <t>Email</t>
   </si>
@@ -36,10 +36,25 @@
     <t>wiasm.mtour@gmail.com</t>
   </si>
   <si>
-    <t>wiasm.mtourgmail.com</t>
-  </si>
-  <si>
-    <t>wiasm.mtour@gmail</t>
+    <t>Test Case</t>
+  </si>
+  <si>
+    <t>Run</t>
+  </si>
+  <si>
+    <t>Check response on entering valid  Credentials(Email and password)</t>
+  </si>
+  <si>
+    <t>asdas</t>
+  </si>
+  <si>
+    <t>asd</t>
+  </si>
+  <si>
+    <t>retyertetertert</t>
+  </si>
+  <si>
+    <t>rterterter</t>
   </si>
 </sst>
 </file>
@@ -407,65 +422,96 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{894A201A-8780-486E-9C0F-F30362CF720D}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:XFD33"/>
+      <selection activeCell="A6" sqref="A6:XFD36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="54.85546875" customWidth="1"/>
-    <col min="2" max="2" width="53.42578125" customWidth="1"/>
+    <col min="2" max="2" width="63.28515625" customWidth="1"/>
+    <col min="3" max="3" width="31.140625" customWidth="1"/>
+    <col min="4" max="4" width="38.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="1">
+      <c r="D2" s="1">
         <v>123456789</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="1">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
         <v>1</v>
       </c>
+      <c r="B3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>1</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="1">
+      <c r="D4" s="1">
+        <v>123456789</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="1">
-        <v>123456789</v>
+      <c r="B5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="1">
+        <v>25121</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{DFC47654-6558-471F-A83D-54AE31C0BDA7}"/>
-    <hyperlink ref="A3" r:id="rId2" display="wiasm.mtour@gmail.com" xr:uid="{4CEEEF5D-0748-4D12-B2E9-6779B96339FC}"/>
-    <hyperlink ref="A4" r:id="rId3" xr:uid="{ECB027C1-3FC3-4F56-94A9-F65C87643A19}"/>
-    <hyperlink ref="A5" r:id="rId4" xr:uid="{42D61707-9562-47EA-BE95-23F0C6A0D8C8}"/>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{B1DBD8EC-CA61-4160-844E-1DCFD99B15A1}"/>
+    <hyperlink ref="C4" r:id="rId2" xr:uid="{957BFC01-0302-4490-8D63-E4214AF5C2F9}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
summary,passed and failed reports
</commit_message>
<xml_diff>
--- a/files/ConduitLoginTest.xlsx
+++ b/files/ConduitLoginTest.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="10">
   <si>
     <t>Email</t>
   </si>
@@ -47,19 +47,13 @@
     <t>asdas</t>
   </si>
   <si>
-    <t>asd</t>
-  </si>
-  <si>
     <t>retyertetertert</t>
   </si>
   <si>
-    <t>rterterter</t>
-  </si>
-  <si>
     <t>wesam</t>
   </si>
   <si>
-    <t>wesa</t>
+    <t>Test Case Number</t>
   </si>
 </sst>
 </file>
@@ -427,110 +421,125 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:XFD52"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5:E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="54.85546875" customWidth="1"/>
     <col min="2" max="2" width="63.28515625" customWidth="1"/>
-    <col min="3" max="3" width="31.140625" customWidth="1"/>
+    <col min="3" max="3" width="68.7109375" customWidth="1"/>
     <col min="4" max="4" width="38.5703125" customWidth="1"/>
+    <col min="5" max="5" width="29.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="2">
+        <v>0</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="1">
+      <c r="E2" s="1">
         <v>123456789</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="1">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" s="1">
+        <v>123456789</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>1</v>
+      </c>
+      <c r="B4" s="2">
+        <v>2</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" s="1">
+        <v>123456789</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>1</v>
+      </c>
+      <c r="B5" s="1">
+        <v>3</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>7</v>
+      <c r="D5" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E5" s="1">
+        <v>123456789</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="2">
-        <v>1</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="2" t="s">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>1</v>
+      </c>
+      <c r="B6" s="2">
+        <v>4</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="1">
+      <c r="E6" s="1">
         <v>123456789</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
-        <v>1</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" s="1">
-        <v>25121</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="2">
-        <v>1</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D6" t="s">
-        <v>11</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1"/>
-    <hyperlink ref="C4" r:id="rId2"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
summary ,passed, skipped, failed reports
</commit_message>
<xml_diff>
--- a/files/ConduitLoginTest.xlsx
+++ b/files/ConduitLoginTest.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="19">
   <si>
     <t>Email</t>
   </si>
@@ -35,25 +35,52 @@
     <t>wiasm.mtour@gmail.com</t>
   </si>
   <si>
-    <t>Test Case</t>
-  </si>
-  <si>
     <t>Run</t>
   </si>
   <si>
     <t>Check response on entering valid  Credentials(Email and password)</t>
   </si>
   <si>
-    <t>asdas</t>
-  </si>
-  <si>
-    <t>retyertetertert</t>
-  </si>
-  <si>
-    <t>wesam</t>
-  </si>
-  <si>
     <t>Test Case Number</t>
+  </si>
+  <si>
+    <t>wiasm.mtour@gmail.</t>
+  </si>
+  <si>
+    <t>Check response on entering invalid Email and valid  password</t>
+  </si>
+  <si>
+    <t>Check response on entering valid Email and invalid password</t>
+  </si>
+  <si>
+    <t>Check response on entering valid Email and blank  password</t>
+  </si>
+  <si>
+    <t>Check response on entering blank Email and vaild  password</t>
+  </si>
+  <si>
+    <t>test case number 1</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>test case number 2</t>
+  </si>
+  <si>
+    <t>test case number 3</t>
+  </si>
+  <si>
+    <t>test case number 4</t>
+  </si>
+  <si>
+    <t>test case number 5</t>
+  </si>
+  <si>
+    <t>discerption</t>
   </si>
 </sst>
 </file>
@@ -423,8 +450,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5:E6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -438,13 +465,13 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>0</v>
@@ -454,14 +481,14 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="2">
-        <v>1</v>
-      </c>
-      <c r="B2" s="2">
-        <v>0</v>
+      <c r="A2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>11</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>2</v>
@@ -471,75 +498,72 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
-        <v>1</v>
-      </c>
-      <c r="B3" s="1">
-        <v>1</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>6</v>
+      <c r="A3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>2</v>
       </c>
       <c r="E3" s="1">
-        <v>123456789</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="2">
-        <v>1</v>
-      </c>
-      <c r="B4" s="2">
-        <v>2</v>
+      <c r="A4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>15</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="E4" s="1">
         <v>123456789</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
-        <v>1</v>
-      </c>
-      <c r="B5" s="1">
-        <v>3</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>7</v>
+      <c r="A5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>9</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E5" s="1">
-        <v>123456789</v>
-      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="2">
-        <v>1</v>
-      </c>
-      <c r="B6" s="2">
-        <v>4</v>
+      <c r="A6" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>17</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="E6" s="1">
         <v>123456789</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D4" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>